<commit_message>
New files to upload
</commit_message>
<xml_diff>
--- a/actuals.xlsx
+++ b/actuals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diksha.a.singh\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75C34A1-2DE8-4D74-A4F8-B0A826FCA2CF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDD8618-E254-4E17-A326-814D0FCFA286}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA29AD36-3365-4DBB-B94A-66709C8A5AF5}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Amt Of Claims</t>
-  </si>
-  <si>
     <t>General Insurance</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Personal Accident</t>
+  </si>
+  <si>
+    <t>No. of Policies</t>
   </si>
 </sst>
 </file>
@@ -165,21 +165,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -191,6 +182,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -507,7 +501,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D22733-6E3B-4F52-BEC3-9693A70FDEAF}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -524,146 +518,1406 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2">
+        <v>38503</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="8">
+        <v>36196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="8">
+        <v>9927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="8">
+        <v>51169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="8">
+        <v>36356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3">
-        <v>155000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="5" t="s">
+      <c r="D7" s="8">
+        <v>48900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="8">
+        <v>29795</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="8">
+        <v>49313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="8">
+        <v>45410</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="8">
+        <v>26214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="8">
+        <v>55392</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="8">
+        <v>38498</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="8">
+        <v>32743</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="8">
+        <v>10528</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="8">
+        <v>16422</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="8">
+        <v>31558</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="8">
+        <v>57253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="8">
+        <v>38884</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="8">
+        <v>48994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4">
-        <v>555000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="5" t="s">
+      <c r="D21" s="8">
+        <v>21602</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="8">
+        <v>35079</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="8">
+        <v>57253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="8">
+        <v>51266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="8">
+        <v>36161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="8">
+        <v>57638</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="8">
+        <v>43907</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="8">
+        <v>59815</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="8">
+        <v>51360</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="8">
+        <v>34215</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="4"/>
+      <c r="B31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4">
-        <v>420000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
-      <c r="B5" s="10" t="s">
+      <c r="C31" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="8">
+        <v>18340</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="8">
+        <v>9922</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="8">
+        <v>46855</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="8">
+        <v>46048</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="8">
+        <v>43044</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="8">
+        <v>36196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="8">
+        <v>38498</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="8">
+        <v>32001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="8">
+        <v>9922</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="8">
+        <v>21539</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="8">
+        <v>25120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="8">
+        <v>55361</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="8">
+        <v>11911</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="8">
+        <v>59270</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="8">
+        <v>4771</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="8">
+        <v>36647</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="8">
+        <v>59395</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="8">
+        <v>23329</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="8">
+        <v>2275</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="8">
+        <v>9927</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="8">
+        <v>7110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="8">
+        <v>52672</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="8">
+        <v>49638</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="8">
+        <v>31558</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="8">
+        <v>23168</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="8">
+        <v>57253</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="8">
+        <v>16935</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="8">
+        <v>16128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="8">
+        <v>29287</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="8">
+        <v>26214</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="8">
+        <v>28007</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="8">
+        <v>54176</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="8">
+        <v>26784</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="8">
+        <v>32420</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="8">
+        <v>27589</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="8">
+        <v>12160</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="8">
+        <v>44003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="8">
+        <v>29795</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="8">
+        <v>22563</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="8">
+        <v>50471</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="8">
+        <v>12160</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="8">
+        <v>10695</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="8">
+        <v>30976</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="8">
+        <v>9344</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="8">
+        <v>32420</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="8">
+        <v>47749</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="8">
+        <v>36134</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="8">
+        <v>27363</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="8">
+        <v>26688</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="8">
+        <v>28455</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="8">
+        <v>52098</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="8">
+        <v>43044</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="8">
+        <v>51266</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="8">
+        <v>24993</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="4"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="8">
+        <v>28007</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="4"/>
+      <c r="B86" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C86" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" s="8">
+        <v>48544</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="8">
+        <v>3042</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="8">
+        <v>20071</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="8">
+        <v>36647</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="8">
+        <v>57606</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="8">
+        <v>13280</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4">
-        <v>220000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="5" t="s">
+      <c r="D92" s="8">
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="8">
+        <v>35238</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="8">
+        <v>9922</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="8">
+        <v>17859</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="8">
+        <v>6182</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="8">
+        <v>19010</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="8">
+        <v>29287</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="8">
+        <v>24966</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="8">
+        <v>27363</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="8">
+        <v>59270</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="8">
+        <v>50055</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="8">
+        <v>38118</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="8">
+        <v>11777</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="8">
+        <v>48900</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="8">
+        <v>27589</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="8">
+        <v>23329</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="8">
+        <v>49313</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="8">
+        <v>11841</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="8">
+        <v>20292</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="8">
+        <v>43844</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="8">
+        <v>18340</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="8">
+        <v>57638</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="4"/>
+      <c r="B114" s="4"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="8">
+        <v>57253</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="4"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="8">
+        <v>28165</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="4"/>
+      <c r="B116" s="4"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="8">
+        <v>46048</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="4"/>
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="8">
+        <v>50145</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="8">
+        <v>59585</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="8">
+        <v>47136</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="8">
+        <v>28007</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="8">
+        <v>50759</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="4"/>
+      <c r="B122" s="4"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="8">
+        <v>28455</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="4"/>
+      <c r="B123" s="4"/>
+      <c r="C123" s="4"/>
+      <c r="D123" s="8">
+        <v>44517</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="4"/>
+      <c r="B124" s="4"/>
+      <c r="C124" s="4"/>
+      <c r="D124" s="8">
+        <v>51266</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="4"/>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="8">
+        <v>24193</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A126" s="4"/>
+      <c r="B126" s="4"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="8">
+        <v>33126</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="4"/>
+      <c r="B127" s="4"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="8">
+        <v>20967</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="4"/>
+      <c r="B128" s="4"/>
+      <c r="C128" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4">
-        <v>1050000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4">
-        <v>360000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
-      <c r="B8" s="10" t="s">
+      <c r="D128" s="8">
+        <v>6182</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A129" s="4"/>
+      <c r="B129" s="4"/>
+      <c r="C129" s="4"/>
+      <c r="D129" s="8">
+        <v>52867</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="4"/>
+      <c r="B130" s="4"/>
+      <c r="C130" s="4"/>
+      <c r="D130" s="8">
+        <v>58147</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="4"/>
+      <c r="B131" s="4"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="8">
+        <v>57600</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="4"/>
+      <c r="B132" s="4"/>
+      <c r="C132" s="4"/>
+      <c r="D132" s="8">
+        <v>11841</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A133" s="4"/>
+      <c r="B133" s="4"/>
+      <c r="C133" s="4"/>
+      <c r="D133" s="8">
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A134" s="4"/>
+      <c r="B134" s="4"/>
+      <c r="C134" s="4"/>
+      <c r="D134" s="8">
+        <v>57253</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A135" s="4"/>
+      <c r="B135" s="4"/>
+      <c r="C135" s="4"/>
+      <c r="D135" s="8">
+        <v>32001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A136" s="4"/>
+      <c r="B136" s="4"/>
+      <c r="C136" s="4"/>
+      <c r="D136" s="8">
+        <v>55361</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A137" s="4"/>
+      <c r="B137" s="4"/>
+      <c r="C137" s="4"/>
+      <c r="D137" s="8">
+        <v>38884</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A138" s="4"/>
+      <c r="B138" s="4"/>
+      <c r="C138" s="4"/>
+      <c r="D138" s="8">
+        <v>2976</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A139" s="4"/>
+      <c r="B139" s="4"/>
+      <c r="C139" s="4"/>
+      <c r="D139" s="8">
+        <v>14342</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A140" s="4"/>
+      <c r="B140" s="4"/>
+      <c r="C140" s="4"/>
+      <c r="D140" s="8">
+        <v>9344</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A141" s="4"/>
+      <c r="B141" s="4"/>
+      <c r="C141" s="4"/>
+      <c r="D141" s="8">
+        <v>11491</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A142" s="4"/>
+      <c r="B142" s="4"/>
+      <c r="C142" s="4"/>
+      <c r="D142" s="8">
+        <v>25120</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A143" s="4"/>
+      <c r="B143" s="5"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="8">
+        <v>24193</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A144" s="4"/>
+      <c r="B144" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C144" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D144" s="8">
+        <v>13280</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A145" s="4"/>
+      <c r="B145" s="4"/>
+      <c r="C145" s="4"/>
+      <c r="D145" s="8">
+        <v>20967</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A146" s="4"/>
+      <c r="B146" s="4"/>
+      <c r="C146" s="5"/>
+      <c r="D146" s="8">
+        <v>35040</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A147" s="4"/>
+      <c r="B147" s="4"/>
+      <c r="C147" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="4">
-        <v>220000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="5" t="s">
+      <c r="D147" s="8">
+        <v>36356</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A148" s="4"/>
+      <c r="B148" s="4"/>
+      <c r="C148" s="4"/>
+      <c r="D148" s="8">
+        <v>23617</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A149" s="4"/>
+      <c r="B149" s="4"/>
+      <c r="C149" s="4"/>
+      <c r="D149" s="8">
+        <v>26784</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="4"/>
+      <c r="B150" s="4"/>
+      <c r="C150" s="4"/>
+      <c r="D150" s="8">
+        <v>55392</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A151" s="4"/>
+      <c r="B151" s="4"/>
+      <c r="C151" s="4"/>
+      <c r="D151" s="8">
+        <v>23235</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A152" s="4"/>
+      <c r="B152" s="4"/>
+      <c r="C152" s="4"/>
+      <c r="D152" s="8">
+        <v>49538</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="4"/>
+      <c r="B153" s="4"/>
+      <c r="C153" s="4"/>
+      <c r="D153" s="8">
+        <v>10183</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A154" s="4"/>
+      <c r="B154" s="4"/>
+      <c r="C154" s="4"/>
+      <c r="D154" s="8">
+        <v>9927</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A155" s="4"/>
+      <c r="B155" s="4"/>
+      <c r="C155" s="4"/>
+      <c r="D155" s="8">
+        <v>57447</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="4"/>
+      <c r="B156" s="4"/>
+      <c r="C156" s="4"/>
+      <c r="D156" s="8">
+        <v>38503</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="4"/>
+      <c r="B157" s="4"/>
+      <c r="C157" s="4"/>
+      <c r="D157" s="8">
+        <v>35079</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A158" s="4"/>
+      <c r="B158" s="4"/>
+      <c r="C158" s="4"/>
+      <c r="D158" s="8">
+        <v>22881</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A159" s="4"/>
+      <c r="B159" s="4"/>
+      <c r="C159" s="4"/>
+      <c r="D159" s="8">
+        <v>28390</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A160" s="4"/>
+      <c r="B160" s="4"/>
+      <c r="C160" s="4"/>
+      <c r="D160" s="8">
+        <v>5799</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A161" s="4"/>
+      <c r="B161" s="4"/>
+      <c r="C161" s="4"/>
+      <c r="D161" s="8">
+        <v>57638</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A162" s="4"/>
+      <c r="B162" s="4"/>
+      <c r="C162" s="4"/>
+      <c r="D162" s="8">
+        <v>10371</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A163" s="4"/>
+      <c r="B163" s="4"/>
+      <c r="C163" s="4"/>
+      <c r="D163" s="8">
+        <v>33126</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A164" s="4"/>
+      <c r="B164" s="4"/>
+      <c r="C164" s="5"/>
+      <c r="D164" s="8">
+        <v>58688</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A165" s="4"/>
+      <c r="B165" s="4"/>
+      <c r="C165" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="4">
-        <v>1270000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="4">
-        <v>492500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="4">
-        <v>600000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="4">
-        <v>170000</v>
+      <c r="D165" s="8">
+        <v>11491</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A166" s="4"/>
+      <c r="B166" s="4"/>
+      <c r="C166" s="4"/>
+      <c r="D166" s="8">
+        <v>49477</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A167" s="4"/>
+      <c r="B167" s="4"/>
+      <c r="C167" s="4"/>
+      <c r="D167" s="8">
+        <v>57600</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A168" s="4"/>
+      <c r="B168" s="4"/>
+      <c r="C168" s="4"/>
+      <c r="D168" s="8">
+        <v>41122</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A169" s="5"/>
+      <c r="B169" s="5"/>
+      <c r="C169" s="5"/>
+      <c r="D169" s="8">
+        <v>13702</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
+  <mergeCells count="17">
+    <mergeCell ref="C86:C91"/>
+    <mergeCell ref="C92:C127"/>
+    <mergeCell ref="C128:C143"/>
+    <mergeCell ref="B144:B169"/>
+    <mergeCell ref="C144:C146"/>
+    <mergeCell ref="C147:C164"/>
+    <mergeCell ref="C165:C169"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="C7:C20"/>
+    <mergeCell ref="C21:C30"/>
+    <mergeCell ref="B31:B85"/>
+    <mergeCell ref="C31:C38"/>
+    <mergeCell ref="C39:C70"/>
+    <mergeCell ref="C71:C85"/>
+    <mergeCell ref="A2:A169"/>
+    <mergeCell ref="B2:B30"/>
+    <mergeCell ref="B86:B143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>